<commit_message>
Design finish version 2
</commit_message>
<xml_diff>
--- a/design-document/ScreenClassManagement.xlsx
+++ b/design-document/ScreenClassManagement.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10547" tabRatio="833" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10547" tabRatio="833"/>
   </bookViews>
   <sheets>
     <sheet name="01_Screen Layout" sheetId="4" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="05_Check Condition" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'01_Screen Layout'!$A$1:$K$27</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'01_Screen Layout'!$A$1:$N$44</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'02_Item Definition'!$A$1:$K$14</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'03_Definition'!$A$1:$V$22</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'04_check Condition Monadic'!$A$1:$J$15</definedName>
@@ -1076,6 +1076,195 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1085,15 +1274,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1105,189 +1288,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2118,7 +2118,7 @@
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="15240"/>
-          <a:ext cx="9491133" cy="502920"/>
+          <a:ext cx="8932333" cy="502920"/>
           <a:chOff x="0" y="2"/>
           <a:chExt cx="1121" cy="52"/>
         </a:xfrm>
@@ -2768,17 +2768,22 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>304799</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>50801</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="8157210" cy="2042160"/>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>880532</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>131234</xdr:rowOff>
+    </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="Picture 1"/>
+        <xdr:cNvPr id="24" name="Picture 23"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2791,46 +2796,77 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="53340" y="1148715"/>
-          <a:ext cx="8157210" cy="2042160"/>
+          <a:off x="990599" y="753534"/>
+          <a:ext cx="7391400" cy="5981700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>313267</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>59267</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>821266</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="Rectangle 25"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="999067" y="762000"/>
+          <a:ext cx="7323666" cy="5969000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
       </xdr:spPr>
-    </xdr:pic>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
-  </xdr:oneCellAnchor>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6547,15 +6583,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.35"/>
   <cols>
     <col min="1" max="9" width="9" style="1"/>
     <col min="10" max="10" width="17.44140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="26.109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18.77734375" style="1" customWidth="1"/>
     <col min="12" max="12" width="0.33203125" style="1" hidden="1" customWidth="1"/>
     <col min="13" max="14" width="9" style="1" hidden="1" customWidth="1"/>
     <col min="15" max="16384" width="9" style="1"/>
@@ -7044,95 +7080,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15" customHeight="1">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="87" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="66"/>
+      <c r="B1" s="88"/>
       <c r="C1" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="88" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66" t="s">
+      <c r="E1" s="88"/>
+      <c r="F1" s="88" t="s">
         <v>84</v>
       </c>
-      <c r="G1" s="66"/>
-      <c r="H1" s="67" t="s">
+      <c r="G1" s="88"/>
+      <c r="H1" s="112" t="s">
         <v>83</v>
       </c>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="68"/>
+      <c r="I1" s="112"/>
+      <c r="J1" s="112"/>
+      <c r="K1" s="112"/>
+      <c r="L1" s="113"/>
     </row>
     <row r="2" spans="1:22" ht="15" customHeight="1">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="89" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="69" t="s">
+      <c r="B2" s="90"/>
+      <c r="C2" s="98" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="70"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="72" t="s">
+      <c r="D2" s="99"/>
+      <c r="E2" s="114"/>
+      <c r="F2" s="90" t="s">
         <v>80</v>
       </c>
-      <c r="G2" s="72"/>
-      <c r="H2" s="69" t="s">
+      <c r="G2" s="90"/>
+      <c r="H2" s="98" t="s">
         <v>79</v>
       </c>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="81"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="100"/>
     </row>
     <row r="3" spans="1:22" ht="45.35" customHeight="1">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="91" t="s">
         <v>78</v>
       </c>
-      <c r="B3" s="77"/>
-      <c r="C3" s="57" t="s">
+      <c r="B3" s="92"/>
+      <c r="C3" s="95" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="80"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="97"/>
     </row>
     <row r="4" spans="1:22" ht="15" customHeight="1" thickBot="1">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="93" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="79"/>
-      <c r="C4" s="83"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="84"/>
-      <c r="H4" s="84"/>
-      <c r="I4" s="84"/>
-      <c r="J4" s="84"/>
-      <c r="K4" s="84"/>
-      <c r="L4" s="85"/>
+      <c r="B4" s="94"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="103"/>
+      <c r="E4" s="103"/>
+      <c r="F4" s="103"/>
+      <c r="G4" s="103"/>
+      <c r="H4" s="103"/>
+      <c r="I4" s="103"/>
+      <c r="J4" s="103"/>
+      <c r="K4" s="103"/>
+      <c r="L4" s="104"/>
     </row>
     <row r="5" spans="1:22">
-      <c r="A5" s="73"/>
-      <c r="B5" s="73"/>
+      <c r="A5" s="86"/>
+      <c r="B5" s="86"/>
     </row>
     <row r="6" spans="1:22" ht="13.35">
-      <c r="A6" s="82" t="s">
+      <c r="A6" s="101" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="82"/>
-      <c r="C6" s="82"/>
+      <c r="B6" s="101"/>
+      <c r="C6" s="101"/>
       <c r="N6" s="44" t="s">
         <v>102</v>
       </c>
@@ -7141,38 +7177,38 @@
       <c r="A8" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="64" t="s">
+      <c r="B8" s="105" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="64" t="s">
+      <c r="C8" s="106"/>
+      <c r="D8" s="106"/>
+      <c r="E8" s="105" t="s">
         <v>69</v>
       </c>
-      <c r="F8" s="65"/>
-      <c r="G8" s="65"/>
-      <c r="H8" s="65"/>
-      <c r="I8" s="65"/>
-      <c r="J8" s="65"/>
-      <c r="K8" s="65"/>
-      <c r="L8" s="65"/>
-      <c r="N8" s="89" t="s">
+      <c r="F8" s="106"/>
+      <c r="G8" s="106"/>
+      <c r="H8" s="106"/>
+      <c r="I8" s="106"/>
+      <c r="J8" s="106"/>
+      <c r="K8" s="106"/>
+      <c r="L8" s="106"/>
+      <c r="N8" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="O8" s="89" t="s">
+      <c r="O8" s="81" t="s">
         <v>88</v>
       </c>
-      <c r="P8" s="91" t="s">
+      <c r="P8" s="83" t="s">
         <v>103</v>
       </c>
-      <c r="Q8" s="92"/>
-      <c r="R8" s="92"/>
-      <c r="S8" s="92"/>
-      <c r="T8" s="93"/>
-      <c r="U8" s="89" t="s">
+      <c r="Q8" s="84"/>
+      <c r="R8" s="84"/>
+      <c r="S8" s="84"/>
+      <c r="T8" s="85"/>
+      <c r="U8" s="81" t="s">
         <v>104</v>
       </c>
-      <c r="V8" s="89" t="s">
+      <c r="V8" s="81" t="s">
         <v>89</v>
       </c>
     </row>
@@ -7180,34 +7216,34 @@
       <c r="A9" s="35">
         <v>1</v>
       </c>
-      <c r="B9" s="88" t="s">
+      <c r="B9" s="109" t="s">
         <v>74</v>
       </c>
-      <c r="C9" s="87"/>
-      <c r="D9" s="87"/>
-      <c r="E9" s="62" t="s">
+      <c r="C9" s="108"/>
+      <c r="D9" s="108"/>
+      <c r="E9" s="110" t="s">
         <v>73</v>
       </c>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="63"/>
-      <c r="I9" s="63"/>
-      <c r="J9" s="63"/>
-      <c r="K9" s="63"/>
-      <c r="L9" s="63"/>
-      <c r="N9" s="90"/>
-      <c r="O9" s="90"/>
-      <c r="P9" s="91" t="s">
+      <c r="F9" s="111"/>
+      <c r="G9" s="111"/>
+      <c r="H9" s="111"/>
+      <c r="I9" s="111"/>
+      <c r="J9" s="111"/>
+      <c r="K9" s="111"/>
+      <c r="L9" s="111"/>
+      <c r="N9" s="82"/>
+      <c r="O9" s="82"/>
+      <c r="P9" s="83" t="s">
         <v>105</v>
       </c>
-      <c r="Q9" s="92"/>
+      <c r="Q9" s="84"/>
       <c r="R9" s="45"/>
-      <c r="S9" s="91" t="s">
+      <c r="S9" s="83" t="s">
         <v>106</v>
       </c>
-      <c r="T9" s="93"/>
-      <c r="U9" s="90"/>
-      <c r="V9" s="90"/>
+      <c r="T9" s="85"/>
+      <c r="U9" s="82"/>
+      <c r="V9" s="82"/>
     </row>
     <row r="10" spans="1:22" ht="36.85" customHeight="1">
       <c r="E10" s="37"/>
@@ -7217,277 +7253,277 @@
       <c r="O10" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="P10" s="97" t="s">
+      <c r="P10" s="76" t="s">
         <v>108</v>
       </c>
-      <c r="Q10" s="98"/>
-      <c r="R10" s="99"/>
-      <c r="S10" s="100" t="s">
+      <c r="Q10" s="77"/>
+      <c r="R10" s="78"/>
+      <c r="S10" s="79" t="s">
         <v>107</v>
       </c>
-      <c r="T10" s="101"/>
-      <c r="U10" s="102" t="s">
+      <c r="T10" s="80"/>
+      <c r="U10" s="52" t="s">
         <v>109</v>
       </c>
-      <c r="V10" s="102" t="s">
+      <c r="V10" s="52" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:22" ht="36.85" customHeight="1">
-      <c r="A11" s="82" t="s">
+      <c r="A11" s="101" t="s">
         <v>72</v>
       </c>
-      <c r="B11" s="82"/>
-      <c r="C11" s="82"/>
-      <c r="N11" s="94">
+      <c r="B11" s="101"/>
+      <c r="C11" s="101"/>
+      <c r="N11" s="73">
         <v>2</v>
       </c>
-      <c r="O11" s="111" t="s">
+      <c r="O11" s="61" t="s">
         <v>113</v>
       </c>
-      <c r="P11" s="114" t="s">
+      <c r="P11" s="64" t="s">
         <v>110</v>
       </c>
-      <c r="Q11" s="115"/>
-      <c r="R11" s="116"/>
-      <c r="S11" s="105"/>
-      <c r="T11" s="106"/>
-      <c r="U11" s="103"/>
-      <c r="V11" s="103"/>
+      <c r="Q11" s="65"/>
+      <c r="R11" s="66"/>
+      <c r="S11" s="55"/>
+      <c r="T11" s="56"/>
+      <c r="U11" s="53"/>
+      <c r="V11" s="53"/>
     </row>
     <row r="12" spans="1:22" ht="37.35" customHeight="1">
-      <c r="N12" s="95"/>
-      <c r="O12" s="112"/>
-      <c r="P12" s="117"/>
-      <c r="Q12" s="118"/>
-      <c r="R12" s="119"/>
-      <c r="S12" s="107"/>
-      <c r="T12" s="108"/>
-      <c r="U12" s="103"/>
-      <c r="V12" s="103"/>
+      <c r="N12" s="74"/>
+      <c r="O12" s="62"/>
+      <c r="P12" s="67"/>
+      <c r="Q12" s="68"/>
+      <c r="R12" s="69"/>
+      <c r="S12" s="57"/>
+      <c r="T12" s="58"/>
+      <c r="U12" s="53"/>
+      <c r="V12" s="53"/>
     </row>
     <row r="13" spans="1:22" ht="12.7" customHeight="1">
       <c r="A13" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="64" t="s">
+      <c r="B13" s="105" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="65"/>
-      <c r="D13" s="65"/>
-      <c r="E13" s="64" t="s">
+      <c r="C13" s="106"/>
+      <c r="D13" s="106"/>
+      <c r="E13" s="105" t="s">
         <v>69</v>
       </c>
-      <c r="F13" s="65"/>
-      <c r="G13" s="65"/>
-      <c r="H13" s="65"/>
-      <c r="I13" s="65"/>
-      <c r="J13" s="65"/>
-      <c r="K13" s="65"/>
-      <c r="L13" s="65"/>
-      <c r="N13" s="95"/>
-      <c r="O13" s="112"/>
-      <c r="P13" s="117"/>
-      <c r="Q13" s="118"/>
-      <c r="R13" s="119"/>
-      <c r="S13" s="107"/>
-      <c r="T13" s="108"/>
-      <c r="U13" s="103"/>
-      <c r="V13" s="103"/>
+      <c r="F13" s="106"/>
+      <c r="G13" s="106"/>
+      <c r="H13" s="106"/>
+      <c r="I13" s="106"/>
+      <c r="J13" s="106"/>
+      <c r="K13" s="106"/>
+      <c r="L13" s="106"/>
+      <c r="N13" s="74"/>
+      <c r="O13" s="62"/>
+      <c r="P13" s="67"/>
+      <c r="Q13" s="68"/>
+      <c r="R13" s="69"/>
+      <c r="S13" s="57"/>
+      <c r="T13" s="58"/>
+      <c r="U13" s="53"/>
+      <c r="V13" s="53"/>
     </row>
     <row r="14" spans="1:22" ht="31.5" customHeight="1">
       <c r="A14" s="35">
         <v>1</v>
       </c>
-      <c r="B14" s="86" t="s">
+      <c r="B14" s="107" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="87"/>
-      <c r="D14" s="87"/>
-      <c r="E14" s="57" t="s">
+      <c r="C14" s="108"/>
+      <c r="D14" s="108"/>
+      <c r="E14" s="95" t="s">
         <v>67</v>
       </c>
-      <c r="F14" s="55"/>
-      <c r="G14" s="55"/>
-      <c r="H14" s="55"/>
-      <c r="I14" s="55"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="55"/>
-      <c r="L14" s="56"/>
-      <c r="N14" s="96"/>
-      <c r="O14" s="113"/>
-      <c r="P14" s="120"/>
-      <c r="Q14" s="121"/>
-      <c r="R14" s="122"/>
-      <c r="S14" s="107"/>
-      <c r="T14" s="108"/>
-      <c r="U14" s="103"/>
-      <c r="V14" s="103"/>
+      <c r="F14" s="96"/>
+      <c r="G14" s="96"/>
+      <c r="H14" s="96"/>
+      <c r="I14" s="96"/>
+      <c r="J14" s="96"/>
+      <c r="K14" s="96"/>
+      <c r="L14" s="118"/>
+      <c r="N14" s="75"/>
+      <c r="O14" s="63"/>
+      <c r="P14" s="70"/>
+      <c r="Q14" s="71"/>
+      <c r="R14" s="72"/>
+      <c r="S14" s="57"/>
+      <c r="T14" s="58"/>
+      <c r="U14" s="53"/>
+      <c r="V14" s="53"/>
     </row>
     <row r="15" spans="1:22" ht="39.35" customHeight="1">
       <c r="A15" s="35">
         <v>2</v>
       </c>
-      <c r="B15" s="58" t="s">
+      <c r="B15" s="119" t="s">
         <v>116</v>
       </c>
-      <c r="C15" s="59"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="61" t="s">
+      <c r="C15" s="120"/>
+      <c r="D15" s="121"/>
+      <c r="E15" s="122" t="s">
         <v>114</v>
       </c>
-      <c r="F15" s="55"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="55"/>
-      <c r="I15" s="55"/>
-      <c r="J15" s="55"/>
-      <c r="K15" s="55"/>
-      <c r="L15" s="56"/>
-      <c r="N15" s="94">
+      <c r="F15" s="96"/>
+      <c r="G15" s="96"/>
+      <c r="H15" s="96"/>
+      <c r="I15" s="96"/>
+      <c r="J15" s="96"/>
+      <c r="K15" s="96"/>
+      <c r="L15" s="118"/>
+      <c r="N15" s="73">
         <v>3</v>
       </c>
-      <c r="O15" s="111" t="s">
+      <c r="O15" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="P15" s="114" t="s">
+      <c r="P15" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="Q15" s="115"/>
-      <c r="R15" s="116"/>
-      <c r="S15" s="107"/>
-      <c r="T15" s="108"/>
-      <c r="U15" s="103"/>
-      <c r="V15" s="103"/>
+      <c r="Q15" s="65"/>
+      <c r="R15" s="66"/>
+      <c r="S15" s="57"/>
+      <c r="T15" s="58"/>
+      <c r="U15" s="53"/>
+      <c r="V15" s="53"/>
     </row>
     <row r="16" spans="1:22" ht="52" customHeight="1">
       <c r="A16" s="34">
         <v>3</v>
       </c>
-      <c r="B16" s="52" t="s">
+      <c r="B16" s="115" t="s">
         <v>111</v>
       </c>
-      <c r="C16" s="53"/>
-      <c r="D16" s="53"/>
-      <c r="E16" s="54" t="s">
+      <c r="C16" s="116"/>
+      <c r="D16" s="116"/>
+      <c r="E16" s="117" t="s">
         <v>66</v>
       </c>
-      <c r="F16" s="55"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="55"/>
-      <c r="I16" s="55"/>
-      <c r="J16" s="55"/>
-      <c r="K16" s="55"/>
-      <c r="L16" s="56"/>
-      <c r="N16" s="96"/>
-      <c r="O16" s="113"/>
-      <c r="P16" s="120"/>
-      <c r="Q16" s="121"/>
-      <c r="R16" s="122"/>
-      <c r="S16" s="109"/>
-      <c r="T16" s="110"/>
-      <c r="U16" s="103"/>
-      <c r="V16" s="103"/>
+      <c r="F16" s="96"/>
+      <c r="G16" s="96"/>
+      <c r="H16" s="96"/>
+      <c r="I16" s="96"/>
+      <c r="J16" s="96"/>
+      <c r="K16" s="96"/>
+      <c r="L16" s="118"/>
+      <c r="N16" s="75"/>
+      <c r="O16" s="63"/>
+      <c r="P16" s="70"/>
+      <c r="Q16" s="71"/>
+      <c r="R16" s="72"/>
+      <c r="S16" s="59"/>
+      <c r="T16" s="60"/>
+      <c r="U16" s="53"/>
+      <c r="V16" s="53"/>
     </row>
     <row r="17" spans="1:22" ht="64.7" customHeight="1">
       <c r="A17" s="34">
         <v>4</v>
       </c>
-      <c r="B17" s="52" t="s">
+      <c r="B17" s="115" t="s">
         <v>115</v>
       </c>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="54" t="s">
+      <c r="C17" s="116"/>
+      <c r="D17" s="116"/>
+      <c r="E17" s="117" t="s">
         <v>65</v>
       </c>
-      <c r="F17" s="55"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="55"/>
-      <c r="I17" s="55"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="55"/>
-      <c r="L17" s="56"/>
-      <c r="N17" s="94">
+      <c r="F17" s="96"/>
+      <c r="G17" s="96"/>
+      <c r="H17" s="96"/>
+      <c r="I17" s="96"/>
+      <c r="J17" s="96"/>
+      <c r="K17" s="96"/>
+      <c r="L17" s="118"/>
+      <c r="N17" s="73">
         <v>4</v>
       </c>
-      <c r="O17" s="111" t="s">
+      <c r="O17" s="61" t="s">
         <v>115</v>
       </c>
-      <c r="P17" s="114" t="s">
+      <c r="P17" s="64" t="s">
         <v>110</v>
       </c>
-      <c r="Q17" s="115"/>
-      <c r="R17" s="116"/>
-      <c r="S17" s="105"/>
-      <c r="T17" s="106"/>
-      <c r="U17" s="103"/>
-      <c r="V17" s="103"/>
+      <c r="Q17" s="65"/>
+      <c r="R17" s="66"/>
+      <c r="S17" s="55"/>
+      <c r="T17" s="56"/>
+      <c r="U17" s="53"/>
+      <c r="V17" s="53"/>
     </row>
     <row r="18" spans="1:22" ht="64.7" customHeight="1">
-      <c r="N18" s="95"/>
-      <c r="O18" s="112"/>
-      <c r="P18" s="117"/>
-      <c r="Q18" s="118"/>
-      <c r="R18" s="119"/>
-      <c r="S18" s="107"/>
-      <c r="T18" s="108"/>
-      <c r="U18" s="103"/>
-      <c r="V18" s="103"/>
+      <c r="N18" s="74"/>
+      <c r="O18" s="62"/>
+      <c r="P18" s="67"/>
+      <c r="Q18" s="68"/>
+      <c r="R18" s="69"/>
+      <c r="S18" s="57"/>
+      <c r="T18" s="58"/>
+      <c r="U18" s="53"/>
+      <c r="V18" s="53"/>
     </row>
     <row r="19" spans="1:22" ht="15.35" customHeight="1">
-      <c r="N19" s="95"/>
-      <c r="O19" s="112"/>
-      <c r="P19" s="117"/>
-      <c r="Q19" s="118"/>
-      <c r="R19" s="119"/>
-      <c r="S19" s="107"/>
-      <c r="T19" s="108"/>
-      <c r="U19" s="103"/>
-      <c r="V19" s="103"/>
+      <c r="N19" s="74"/>
+      <c r="O19" s="62"/>
+      <c r="P19" s="67"/>
+      <c r="Q19" s="68"/>
+      <c r="R19" s="69"/>
+      <c r="S19" s="57"/>
+      <c r="T19" s="58"/>
+      <c r="U19" s="53"/>
+      <c r="V19" s="53"/>
     </row>
     <row r="20" spans="1:22" ht="15.35" customHeight="1">
-      <c r="N20" s="95"/>
-      <c r="O20" s="112"/>
-      <c r="P20" s="117"/>
-      <c r="Q20" s="118"/>
-      <c r="R20" s="119"/>
-      <c r="S20" s="107"/>
-      <c r="T20" s="108"/>
-      <c r="U20" s="103"/>
-      <c r="V20" s="103"/>
+      <c r="N20" s="74"/>
+      <c r="O20" s="62"/>
+      <c r="P20" s="67"/>
+      <c r="Q20" s="68"/>
+      <c r="R20" s="69"/>
+      <c r="S20" s="57"/>
+      <c r="T20" s="58"/>
+      <c r="U20" s="53"/>
+      <c r="V20" s="53"/>
     </row>
     <row r="21" spans="1:22" ht="11.35" customHeight="1">
-      <c r="N21" s="95"/>
-      <c r="O21" s="112"/>
-      <c r="P21" s="117"/>
-      <c r="Q21" s="118"/>
-      <c r="R21" s="119"/>
-      <c r="S21" s="107"/>
-      <c r="T21" s="108"/>
-      <c r="U21" s="103"/>
-      <c r="V21" s="103"/>
+      <c r="N21" s="74"/>
+      <c r="O21" s="62"/>
+      <c r="P21" s="67"/>
+      <c r="Q21" s="68"/>
+      <c r="R21" s="69"/>
+      <c r="S21" s="57"/>
+      <c r="T21" s="58"/>
+      <c r="U21" s="53"/>
+      <c r="V21" s="53"/>
     </row>
     <row r="22" spans="1:22" ht="14.7" customHeight="1">
-      <c r="A22" s="73"/>
-      <c r="B22" s="73"/>
-      <c r="C22" s="73"/>
-      <c r="D22" s="73"/>
-      <c r="E22" s="73"/>
-      <c r="F22" s="73"/>
-      <c r="G22" s="73"/>
-      <c r="H22" s="73"/>
-      <c r="I22" s="73"/>
-      <c r="J22" s="73"/>
-      <c r="K22" s="73"/>
-      <c r="N22" s="96"/>
-      <c r="O22" s="113"/>
-      <c r="P22" s="120"/>
-      <c r="Q22" s="121"/>
-      <c r="R22" s="122"/>
-      <c r="S22" s="109"/>
-      <c r="T22" s="110"/>
-      <c r="U22" s="104"/>
-      <c r="V22" s="104"/>
+      <c r="A22" s="86"/>
+      <c r="B22" s="86"/>
+      <c r="C22" s="86"/>
+      <c r="D22" s="86"/>
+      <c r="E22" s="86"/>
+      <c r="F22" s="86"/>
+      <c r="G22" s="86"/>
+      <c r="H22" s="86"/>
+      <c r="I22" s="86"/>
+      <c r="J22" s="86"/>
+      <c r="K22" s="86"/>
+      <c r="N22" s="75"/>
+      <c r="O22" s="63"/>
+      <c r="P22" s="70"/>
+      <c r="Q22" s="71"/>
+      <c r="R22" s="72"/>
+      <c r="S22" s="59"/>
+      <c r="T22" s="60"/>
+      <c r="U22" s="54"/>
+      <c r="V22" s="54"/>
     </row>
     <row r="23" spans="1:22">
       <c r="N23" s="48"/>
@@ -7568,28 +7604,20 @@
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="V10:V22"/>
-    <mergeCell ref="S11:T16"/>
-    <mergeCell ref="O11:O14"/>
-    <mergeCell ref="P11:R14"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="P15:R16"/>
-    <mergeCell ref="O17:O22"/>
-    <mergeCell ref="P17:R22"/>
-    <mergeCell ref="S17:T22"/>
-    <mergeCell ref="U10:U22"/>
-    <mergeCell ref="N11:N14"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="N17:N22"/>
-    <mergeCell ref="P10:R10"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="P8:T8"/>
-    <mergeCell ref="U8:U9"/>
-    <mergeCell ref="V8:V9"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:L17"/>
+    <mergeCell ref="E14:L14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E15:L15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:L16"/>
+    <mergeCell ref="E9:L9"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:G2"/>
     <mergeCell ref="A22:K22"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
@@ -7606,20 +7634,28 @@
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="E8:L8"/>
     <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:L9"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:L17"/>
-    <mergeCell ref="E14:L14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E15:L15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:L16"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="P8:T8"/>
+    <mergeCell ref="U8:U9"/>
+    <mergeCell ref="V8:V9"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="N11:N14"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="N17:N22"/>
+    <mergeCell ref="P10:R10"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="V10:V22"/>
+    <mergeCell ref="S11:T16"/>
+    <mergeCell ref="O11:O14"/>
+    <mergeCell ref="P11:R14"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="P15:R16"/>
+    <mergeCell ref="O17:O22"/>
+    <mergeCell ref="P17:R22"/>
+    <mergeCell ref="S17:T22"/>
+    <mergeCell ref="U10:U22"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="47" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -7726,11 +7762,11 @@
         <v>44</v>
       </c>
       <c r="G2" s="27"/>
-      <c r="H2" s="91" t="s">
+      <c r="H2" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="92"/>
-      <c r="J2" s="93"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="85"/>
     </row>
     <row r="3" spans="1:10" ht="24" customHeight="1">
       <c r="A3" s="11" t="s">
@@ -8169,7 +8205,7 @@
   </sheetPr>
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="D6" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="D6" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>

</xml_diff>